<commit_message>
Lots of images & brand new awards tab
</commit_message>
<xml_diff>
--- a/data/awards.xlsx
+++ b/data/awards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CC43E4-1346-4D40-861C-1C286E8AE3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E76C772-3F8A-4F4A-BFEC-AA8EC08E2E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="120">
   <si>
     <t>Season</t>
   </si>
@@ -42,9 +42,6 @@
     <t>TRUFFLE</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Champion</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>LVP</t>
   </si>
   <si>
-    <t>LeVeon Bell</t>
-  </si>
-  <si>
     <t>ELP</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Rashaad Penny</t>
   </si>
   <si>
-    <t>Saquon Barkley</t>
-  </si>
-  <si>
     <t>Cordarelle Patterson</t>
   </si>
   <si>
@@ -279,9 +270,6 @@
     <t>www/graphics/awardlogos/ROY.png</t>
   </si>
   <si>
-    <t>www/graphics/awardlogos/PlayoffsMVP</t>
-  </si>
-  <si>
     <t>www/graphics/awardlogos/LVP.png</t>
   </si>
   <si>
@@ -292,6 +280,111 @@
   </si>
   <si>
     <t>www/graphics/awardlogos/RFS.png</t>
+  </si>
+  <si>
+    <t>LeVeon Bell ($48)</t>
+  </si>
+  <si>
+    <t>James Robinson ($4)</t>
+  </si>
+  <si>
+    <t>Darren Waller $24)</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/CC.png</t>
+  </si>
+  <si>
+    <t>Saquon Barkley ($97)</t>
+  </si>
+  <si>
+    <t>Cordarelle Patterson ($15)</t>
+  </si>
+  <si>
+    <t>Deebo Samuel ($36)</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/GF.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/NN.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/WLW.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/FRR.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/ELP.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/dcook.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/jjefferson.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/akamara.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/jhurts.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/lbell.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/jrobinson.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/dwaller.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/jtaylor.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/jchase.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/nharris.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/rpenny.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/sbarkley.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/cpatterson.png</t>
+  </si>
+  <si>
+    <t>www/graphics/players/dsamuel.png</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>www/graphics/awardlogos/BenchCupMVP.png</t>
+  </si>
+  <si>
+    <t>www/graphics/awardlogos/PlayoffsMVP.png</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>9-5</t>
+  </si>
+  <si>
+    <t>2-12</t>
+  </si>
+  <si>
+    <t>4-10</t>
+  </si>
+  <si>
+    <t>8-5</t>
+  </si>
+  <si>
+    <t>7-6</t>
   </si>
 </sst>
 </file>
@@ -335,12 +428,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,23 +650,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="26" width="10.5" customWidth="1"/>
+    <col min="3" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="27" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -581,1105 +675,1220 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1">
         <v>2020</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1">
         <v>2020</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5" s="1">
         <v>2020</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1">
         <v>2020</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1">
         <v>2020</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="B9" s="1">
         <v>2020</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1">
         <v>2020</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="3">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B11" s="1">
         <v>2020</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B12" s="1">
         <v>2020</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1">
         <v>2020</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="1">
         <v>2020</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>2020</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="1">
         <v>2020</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="1">
         <v>2020</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="1">
         <v>2020</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="1">
         <v>2020</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="1">
         <v>2020</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="1">
         <v>2020</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="1">
         <v>2020</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="1">
         <v>2020</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="1">
         <v>2020</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="1">
         <v>2020</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="1">
         <v>2020</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="1">
         <v>2020</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="1">
         <v>2020</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="1">
         <v>2020</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="1">
         <v>2020</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1">
         <v>2021</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B32" s="1">
         <v>2021</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B33" s="1">
         <v>2021</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B34" s="1">
         <v>2021</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>60</v>
+        <v>94</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1">
         <v>2021</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1">
         <v>2021</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="B37" s="1">
         <v>2021</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="B38" s="1">
         <v>2021</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B39" s="1">
         <v>2021</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G39" s="4">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B40" s="1">
         <v>2021</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G40" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B41" s="1">
         <v>2021</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="1">
         <v>2021</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="1">
         <v>2021</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="1">
         <v>2021</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="1">
         <v>2021</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="1">
         <v>2021</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="1">
         <v>2021</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="1">
         <v>2021</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="1">
         <v>2021</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="1">
         <v>2021</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="1">
         <v>2021</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>73</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="1">
         <v>2021</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="1">
         <v>2021</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D53" s="1"/>
       <c r="E53" s="2" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="1">
         <v>2021</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="2" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="1">
         <v>2021</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D55" s="1"/>
       <c r="E55" s="2" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="1">
         <v>2021</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D56" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G56" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="1">
         <v>2021</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="1">
         <v>2021</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="1">
         <v>2021</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>34</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Tons of reformatting and image resizing
</commit_message>
<xml_diff>
--- a/data/awards.xlsx
+++ b/data/awards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E76C772-3F8A-4F4A-BFEC-AA8EC08E2E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF331C1-9D46-7841-B403-AE9B8C141884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>Rashaad Penny</t>
   </si>
   <si>
-    <t>Cordarelle Patterson</t>
-  </si>
-  <si>
     <t>Deebo Samuel</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>7-6</t>
+  </si>
+  <si>
+    <t>Cordarelle Patterson (FL)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -666,7 +666,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1">
         <v>2020</v>
@@ -699,13 +699,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1">
         <v>2020</v>
@@ -722,13 +722,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -736,7 +736,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
@@ -745,13 +745,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1">
         <v>2020</v>
@@ -768,13 +768,13 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1">
         <v>2020</v>
@@ -791,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
@@ -814,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>20</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1">
         <v>2020</v>
@@ -837,7 +837,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>23</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="1">
         <v>2020</v>
@@ -860,7 +860,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>25</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1">
         <v>2020</v>
@@ -883,10 +883,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1">
         <v>2020</v>
@@ -907,10 +907,10 @@
         <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>18</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1">
         <v>2020</v>
@@ -931,10 +931,10 @@
         <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>34</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1">
         <v>2021</v>
@@ -1297,13 +1297,13 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>54</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1">
         <v>2021</v>
@@ -1320,13 +1320,13 @@
         <v>8</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>44</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1">
         <v>2021</v>
@@ -1343,13 +1343,13 @@
         <v>11</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>29</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="1">
         <v>2021</v>
@@ -1366,13 +1366,13 @@
         <v>57</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>54</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="1">
         <v>2021</v>
@@ -1389,7 +1389,7 @@
         <v>16</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>59</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="1">
         <v>2021</v>
@@ -1412,7 +1412,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>60</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" s="1">
         <v>2021</v>
@@ -1435,7 +1435,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>61</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="1">
         <v>2021</v>
@@ -1458,7 +1458,7 @@
         <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>62</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1">
         <v>2021</v>
@@ -1481,10 +1481,10 @@
         <v>28</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>18</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="1">
         <v>2021</v>
@@ -1505,10 +1505,10 @@
         <v>30</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>21</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1">
         <v>2021</v>
@@ -1529,10 +1529,10 @@
         <v>32</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>21</v>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>26</v>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>18</v>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>18</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>21</v>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>21</v>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>34</v>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>26</v>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>26</v>
@@ -1761,13 +1761,13 @@
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>18</v>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="2" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>21</v>

</xml_diff>